<commit_message>
with updated page objects and tests till order page.
</commit_message>
<xml_diff>
--- a/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
+++ b/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fenixoutdoor-my.sharepoint.com/personal/sayrina_lopes_fenixoutdoor_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salo\git\Globetrot\GlobetrotterDeProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_F25DC773A252ABDACC104835919D6A745ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E84FDBC1-1DC2-46E5-B603-FF384B1BA64E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44067B17-BBD3-4DCF-8CF0-E3C82C82E13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>Username</t>
   </si>
@@ -53,113 +53,202 @@
     <t>Product</t>
   </si>
   <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>tshirt</t>
+  </si>
+  <si>
+    <t>SetPassword</t>
+  </si>
+  <si>
+    <t>FenixQA.Voyado+AT1@gmail.com</t>
+  </si>
+  <si>
+    <t>FenixQA.Voyado+AT2@gmail.com</t>
+  </si>
+  <si>
+    <t>FenixQA.Voyado+AT3@gmail.com</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>Sanity</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>GlobetrotterDe Application</t>
+  </si>
+  <si>
+    <t>Pages Classes</t>
+  </si>
+  <si>
+    <t>TestClasses</t>
+  </si>
+  <si>
+    <t>TestCases</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>IndexPage</t>
+  </si>
+  <si>
+    <t>WebIndexPageTest</t>
+  </si>
+  <si>
+    <t>globetrotterdeLogoTest
+globetrotterdeTitleTest</t>
+  </si>
+  <si>
+    <t>Smoke
+Smoke</t>
+  </si>
+  <si>
+    <t>Logo should be present
+Title should match with expected value</t>
+  </si>
+  <si>
+    <t>LoginPage</t>
+  </si>
+  <si>
+    <t>LoginPageTest</t>
+  </si>
+  <si>
+    <t>loginTest</t>
+  </si>
+  <si>
+    <t>Sanity,Smoke</t>
+  </si>
+  <si>
+    <t>User should be able to login</t>
+  </si>
+  <si>
+    <t>HomePage</t>
+  </si>
+  <si>
+    <t>HomePageTest</t>
+  </si>
+  <si>
+    <t>wishlistTest
+orderHistoryandDetailsTest</t>
+  </si>
+  <si>
+    <t>Wishlist should be displayed
+OrderHistory should be displayed.</t>
+  </si>
+  <si>
+    <t>AccountCreationPage</t>
+  </si>
+  <si>
+    <t>AccountCreationPageTest</t>
+  </si>
+  <si>
+    <t>createAccountTest</t>
+  </si>
+  <si>
+    <t>User should be navigated to account creation page</t>
+  </si>
+  <si>
+    <t>Not Functional Fully.</t>
+  </si>
+  <si>
+    <t>SearchResultPage</t>
+  </si>
+  <si>
+    <t>SearchResultPageTest</t>
+  </si>
+  <si>
+    <t>productAvailabilityTest</t>
+  </si>
+  <si>
+    <t>Search the product and product should be displayed.</t>
+  </si>
+  <si>
+    <t>AddToCartPage</t>
+  </si>
+  <si>
+    <t>AddToCartPageTest</t>
+  </si>
+  <si>
+    <t>addToCartTest</t>
+  </si>
+  <si>
+    <t>Regression,Sanity</t>
+  </si>
+  <si>
+    <t>User should be able to add product to the cart</t>
+  </si>
+  <si>
+    <t>OrderPage</t>
+  </si>
+  <si>
+    <t>OrderPageTest</t>
+  </si>
+  <si>
+    <t>priceTest</t>
+  </si>
+  <si>
+    <t>Validate the price on Order page</t>
+  </si>
+  <si>
+    <t>Page not developed fully or functional yet</t>
+  </si>
+  <si>
+    <t>AddressPage</t>
+  </si>
+  <si>
+    <t>ShippingPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>PaymentPage</t>
+  </si>
+  <si>
+    <t>OrderSummary</t>
+  </si>
+  <si>
+    <t>OrderConfirmationPage</t>
+  </si>
+  <si>
+    <t>EndToEndTest</t>
+  </si>
+  <si>
+    <t>endToEndTest</t>
+  </si>
+  <si>
+    <t>User should be able to order the product</t>
+  </si>
+  <si>
     <t>qty</t>
   </si>
   <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>tshirt</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>SetPassword</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zipcode</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>MobilePhone</t>
-  </si>
-  <si>
-    <t>Mrs</t>
-  </si>
-  <si>
-    <t>TestUser</t>
-  </si>
-  <si>
-    <t>UserTest</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>1985</t>
-  </si>
-  <si>
-    <t>ABCDEF</t>
-  </si>
-  <si>
-    <t>EDFG123</t>
-  </si>
-  <si>
-    <t>San</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>91436</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>8489875678</t>
-  </si>
-  <si>
-    <t>FenixQA.Voyado+AT1@gmail.com</t>
-  </si>
-  <si>
-    <t>FenixQA.Voyado+AT2@gmail.com</t>
-  </si>
-  <si>
-    <t>FenixQA.Voyado+AT3@gmail.com</t>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>Now, after login it is not navigating to home page instead it displays login-success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,26 +279,54 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -243,23 +360,62 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -541,12 +697,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.90625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.453125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -573,7 +989,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -604,12 +1020,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -626,31 +1042,31 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4">
-        <v>2</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -660,22 +1076,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20609894-F8CD-4839-9ADA-92729BA03122}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>10</v>
+      <c r="B1" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1271286</v>
       </c>
     </row>
   </sheetData>
@@ -685,211 +1107,52 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4132A040-C522-41E2-B426-7775DBDDB456}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="8.7265625" style="10"/>
-    <col min="14" max="14" width="11.81640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>37</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{BE186A02-AF4D-48DA-9990-ADA546CAD459}"/>

</xml_diff>

<commit_message>
Regression flow to be executed -Updated almost all files
</commit_message>
<xml_diff>
--- a/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
+++ b/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salo\git\Globetrot\GlobetrotterDeProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44067B17-BBD3-4DCF-8CF0-E3C82C82E13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1137ED6D-4EB4-4EB8-8452-4159D8A4F71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Email" sheetId="3" r:id="rId3"/>
     <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
     <sheet name="SearchProduct" sheetId="5" r:id="rId5"/>
-    <sheet name="AccountCreationData" sheetId="6" r:id="rId6"/>
+    <sheet name="CreditCardDetails" sheetId="7" r:id="rId6"/>
+    <sheet name="AccountCreationData" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t>Username</t>
   </si>
@@ -242,6 +243,27 @@
   </si>
   <si>
     <t>Now, after login it is not navigating to home page instead it displays login-success</t>
+  </si>
+  <si>
+    <t>CCHolderName</t>
+  </si>
+  <si>
+    <t>CCNumber</t>
+  </si>
+  <si>
+    <t>CVC</t>
+  </si>
+  <si>
+    <t>CCExpiryMonth</t>
+  </si>
+  <si>
+    <t>CCExpiryYear</t>
+  </si>
+  <si>
+    <t>Test Automation</t>
+  </si>
+  <si>
+    <t>4111 1111 1111 1111</t>
   </si>
 </sst>
 </file>
@@ -407,14 +429,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -699,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -739,13 +761,13 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
@@ -810,7 +832,7 @@
       <c r="B8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -819,7 +841,7 @@
       <c r="E8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1106,6 +1128,60 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8DAF88-FCD7-4E34-A088-466097B92201}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="8">
+        <v>737</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2030</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4132A040-C522-41E2-B426-7775DBDDB456}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Test data and TestNG  files changes
</commit_message>
<xml_diff>
--- a/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
+++ b/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salo\git\Globetrot\GlobetrotterDeProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1137ED6D-4EB4-4EB8-8452-4159D8A4F71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6D6660-B5F8-4F25-805B-CDE9EECE6A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="Email" sheetId="3" r:id="rId3"/>
     <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
     <sheet name="SearchProduct" sheetId="5" r:id="rId5"/>
-    <sheet name="CreditCardDetails" sheetId="7" r:id="rId6"/>
-    <sheet name="AccountCreationData" sheetId="6" r:id="rId7"/>
+    <sheet name="BillingAddress" sheetId="8" r:id="rId6"/>
+    <sheet name="CreditCardDetails" sheetId="7" r:id="rId7"/>
+    <sheet name="AccountCreationData" sheetId="6" r:id="rId8"/>
+    <sheet name="Prod ID" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>Username</t>
   </si>
@@ -264,12 +266,24 @@
   </si>
   <si>
     <t>4111 1111 1111 1111</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>00076367396</t>
+  </si>
+  <si>
+    <t>03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,7 +396,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -438,6 +452,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1098,28 +1118,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20609894-F8CD-4839-9ADA-92729BA03122}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="8">
-        <v>1271286</v>
       </c>
     </row>
   </sheetData>
@@ -1128,52 +1142,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8DAF88-FCD7-4E34-A088-466097B92201}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788B7B40-119A-446F-945E-4D2B0104CBA6}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="8">
-        <v>737</v>
-      </c>
-      <c r="D2" s="8">
-        <v>3</v>
-      </c>
-      <c r="E2" s="8">
-        <v>2030</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1182,6 +1170,62 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8DAF88-FCD7-4E34-A088-466097B92201}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="29"/>
+    <col min="4" max="4" width="13.81640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="28">
+        <v>737</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="28">
+        <v>2030</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4132A040-C522-41E2-B426-7775DBDDB456}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1239,4 +1283,29 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E64913-BB5C-418B-910E-D77B88FF7D60}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
+        <v>1271286</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
This Commit with Sanity, Smoke and regression suites
</commit_message>
<xml_diff>
--- a/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
+++ b/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salo\git\Globetrot\GlobetrotterDeProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6D6660-B5F8-4F25-805B-CDE9EECE6A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0792F7-17AE-4569-9A7E-E707CFCDEEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="8170" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Size</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>tshirt</t>
   </si>
   <si>
@@ -275,6 +272,9 @@
   </si>
   <si>
     <t>03</t>
+  </si>
+  <si>
+    <t>XL</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -449,15 +449,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -758,7 +761,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="13">
         <v>6</v>
@@ -766,7 +769,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="13">
         <v>3</v>
@@ -774,176 +777,176 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="A4" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="E6" s="21" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>28</v>
       </c>
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="D7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="E7" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="C8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="D8" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>37</v>
-      </c>
       <c r="F8" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="C9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="23" t="s">
         <v>41</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="E11" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="F11" s="13"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="C12" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="23" t="s">
         <v>55</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -953,19 +956,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="D14" s="22"/>
       <c r="E14" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -975,7 +978,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -985,19 +988,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="C17" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="D17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="F17" s="13"/>
     </row>
@@ -1083,18 +1086,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FB271F-8BBA-4ED6-8253-75B5881DCB7B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.7265625" style="34"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>66</v>
+      <c r="B1" s="33" t="s">
+        <v>65</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>7</v>
@@ -1102,17 +1108,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="8">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="32">
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1133,7 +1140,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1151,17 +1158,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1179,44 +1186,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="29"/>
-    <col min="4" max="4" width="13.81640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="28"/>
+    <col min="4" max="4" width="13.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="E1" s="26" t="s">
         <v>72</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="28">
+      <c r="C2" s="27">
         <v>737</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="28">
+      <c r="D2" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="27">
         <v>2030</v>
       </c>
     </row>
@@ -1244,12 +1251,12 @@
         <v>4</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>2</v>
@@ -1257,7 +1264,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1265,7 +1272,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>2</v>
@@ -1289,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E64913-BB5C-418B-910E-D77B88FF7D60}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1297,7 +1304,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated Product Size to be selected
</commit_message>
<xml_diff>
--- a/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
+++ b/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salo\git\Globetrot\GlobetrotterDeProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0792F7-17AE-4569-9A7E-E707CFCDEEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050CF2EB-2DF7-4DA7-B893-C23222301264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="8170" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
     <t>03</t>
   </si>
   <si>
-    <t>XL</t>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update size to XL
</commit_message>
<xml_diff>
--- a/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
+++ b/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salo\git\Globetrot\GlobetrotterDeProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050CF2EB-2DF7-4DA7-B893-C23222301264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC2D03-79E9-4AAC-A0CA-A5EF7F51BDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="8170" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
     <t>03</t>
   </si>
   <si>
-    <t>S</t>
+    <t>XL</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Regression test reduced wait for Order and end to end test
</commit_message>
<xml_diff>
--- a/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
+++ b/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salo\git\Globetrot\GlobetrotterDeProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAAC2D03-79E9-4AAC-A0CA-A5EF7F51BDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424044FE-D93D-4205-A6DD-5E11F9392544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -259,9 +259,6 @@
     <t>CCExpiryYear</t>
   </si>
   <si>
-    <t>Test Automation</t>
-  </si>
-  <si>
     <t>4111 1111 1111 1111</t>
   </si>
   <si>
@@ -275,6 +272,9 @@
   </si>
   <si>
     <t>XL</t>
+  </si>
+  <si>
+    <t>TestAutomation</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FB271F-8BBA-4ED6-8253-75B5881DCB7B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1114,7 +1114,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1163,12 +1163,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1180,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8DAF88-FCD7-4E34-A088-466097B92201}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1212,16 +1212,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>73</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>74</v>
       </c>
       <c r="C2" s="27">
         <v>737</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="27">
         <v>2030</v>

</xml_diff>

<commit_message>
Size xpath replaced with css and testdata
</commit_message>
<xml_diff>
--- a/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
+++ b/GlobetrotterDeProject/src/test/resources/TestData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salo\git\Globetrot\GlobetrotterDeProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B10817-F09D-4C57-9715-4BE9F8C3690F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F61071-4DD9-4708-B642-35E5F2D1A137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,7 @@
     <t>TestAutomation</t>
   </si>
   <si>
-    <t>XS</t>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1111,7 +1111,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>78</v>

</xml_diff>